<commit_message>
Changed Resources in both project and excel files and title
>Changed to Health Plus
>Changed to only Nanda Aung in both Database Design and Implementation
</commit_message>
<xml_diff>
--- a/Project Management Folder/PM GP Project.xlsx
+++ b/Project Management Folder/PM GP Project.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Group Project Git\tech_hunters\GP project Old\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Group Project Git\tech_hunters\Project Management Folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{FB0BE743-1B7E-44AD-BF43-0B870FB352E0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CEC5F5B5-BB77-4280-B04A-70D9F9E76F9B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4920" activeTab="3" xr2:uid="{546837BA-72A9-4216-A943-44EAA931800F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4920" xr2:uid="{546837BA-72A9-4216-A943-44EAA931800F}"/>
   </bookViews>
   <sheets>
     <sheet name="Work Breakdown Structure" sheetId="1" r:id="rId1"/>
@@ -260,9 +260,6 @@
     <t>Document  test results</t>
   </si>
   <si>
-    <t>RomantiQ</t>
-  </si>
-  <si>
     <t>Q</t>
   </si>
   <si>
@@ -289,6 +286,9 @@
   </si>
   <si>
     <t>*</t>
+  </si>
+  <si>
+    <t>Health Plus</t>
   </si>
 </sst>
 </file>
@@ -567,7 +567,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -725,7 +725,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1055,8 +1058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A563BC86-AFA4-42BB-BA7E-B8C076EDD1EC}">
   <dimension ref="B1:BE12"/>
   <sheetViews>
-    <sheetView topLeftCell="AK1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AP16" sqref="AP16"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Y7" sqref="Y7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1123,7 +1126,7 @@
   <sheetData>
     <row r="1" spans="2:57" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="AE1" s="40" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="2:57" x14ac:dyDescent="0.25">
@@ -1562,7 +1565,7 @@
         <v>15</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="3:8" x14ac:dyDescent="0.25">
@@ -1609,7 +1612,7 @@
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C21" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>33</v>
@@ -1618,12 +1621,12 @@
         <v>20</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C22" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>32</v>
@@ -1632,13 +1635,13 @@
         <v>14</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C23" s="3"/>
       <c r="H23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="3:8" x14ac:dyDescent="0.25">
@@ -1654,7 +1657,7 @@
   <dimension ref="C3:J22"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1707,7 +1710,7 @@
         <v>63</v>
       </c>
       <c r="H5" s="45" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I5" s="17"/>
       <c r="J5" s="17"/>
@@ -1749,7 +1752,7 @@
         <v>61</v>
       </c>
       <c r="H7" s="45" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I7" s="17"/>
       <c r="J7" s="17"/>
@@ -1771,7 +1774,7 @@
         <v>61</v>
       </c>
       <c r="H8" s="45" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I8" s="17"/>
       <c r="J8" s="17"/>
@@ -1790,7 +1793,7 @@
         <v>58</v>
       </c>
       <c r="G9" s="44" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="H9" s="50"/>
       <c r="I9" s="17"/>
@@ -1830,7 +1833,7 @@
         <v>44</v>
       </c>
       <c r="G11" s="44" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="H11" s="50"/>
       <c r="I11" s="17"/>
@@ -1873,7 +1876,7 @@
         <v>64</v>
       </c>
       <c r="H13" s="45" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I13" s="17"/>
       <c r="J13" s="49"/>
@@ -1912,7 +1915,7 @@
         <v>47</v>
       </c>
       <c r="G15" s="43" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H15" s="50"/>
       <c r="I15" s="17"/>
@@ -1935,7 +1938,7 @@
         <v>64</v>
       </c>
       <c r="H16" s="50" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I16" s="17"/>
       <c r="J16" s="17"/>
@@ -1951,13 +1954,13 @@
         <v>15</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G17" s="43" t="s">
         <v>63</v>
       </c>
       <c r="H17" s="45" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I17" s="17"/>
       <c r="J17" s="17"/>
@@ -1999,7 +2002,7 @@
         <v>63</v>
       </c>
       <c r="H19" s="45" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I19" s="17"/>
       <c r="J19" s="17"/>
@@ -2026,7 +2029,7 @@
     </row>
     <row r="21" spans="3:10" ht="60" x14ac:dyDescent="0.25">
       <c r="C21" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D21" s="24" t="s">
         <v>33</v>
@@ -2035,20 +2038,20 @@
         <v>20</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G21" s="19" t="s">
         <v>63</v>
       </c>
       <c r="H21" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I21" s="17"/>
       <c r="J21" s="17"/>
     </row>
     <row r="22" spans="3:10" ht="60" x14ac:dyDescent="0.25">
       <c r="C22" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D22" s="24" t="s">
         <v>32</v>
@@ -2057,17 +2060,17 @@
         <v>14</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G22" s="19" t="s">
         <v>63</v>
       </c>
       <c r="H22" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I22" s="17"/>
       <c r="J22" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -2080,8 +2083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5C045AA-EC57-48A4-9B67-F4CDFA710B60}">
   <dimension ref="B1:DZ88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AI69" sqref="AI69"/>
+    <sheetView topLeftCell="A14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R27" sqref="R27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2204,7 +2207,7 @@
   <sheetData>
     <row r="1" spans="2:130" ht="26.25" x14ac:dyDescent="0.25">
       <c r="W1" s="46" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="2:130" x14ac:dyDescent="0.25">
@@ -2584,7 +2587,7 @@
     </row>
     <row r="10" spans="2:130" x14ac:dyDescent="0.25">
       <c r="B10" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="CB10" s="3"/>
       <c r="CC10" s="3"/>
@@ -2666,7 +2669,7 @@
     </row>
     <row r="11" spans="2:130" x14ac:dyDescent="0.25">
       <c r="B11" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="CB11" s="3"/>
       <c r="CC11" s="3"/>
@@ -2844,43 +2847,43 @@
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G14" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H14" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I14" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J14" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K14" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L14" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M14" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N14" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O14" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P14" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q14" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R14" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S14" s="3"/>
       <c r="T14" s="3"/>
@@ -3091,58 +3094,58 @@
       <c r="Q16" s="3"/>
       <c r="R16" s="3"/>
       <c r="S16" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T16" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U16" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V16" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W16" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X16" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y16" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Z16" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AA16" s="2">
-        <v>2</v>
-      </c>
-      <c r="AB16" s="25">
-        <v>2</v>
-      </c>
-      <c r="AC16" s="25">
-        <v>2</v>
-      </c>
-      <c r="AD16" s="25">
-        <v>2</v>
-      </c>
-      <c r="AE16" s="25">
-        <v>2</v>
-      </c>
-      <c r="AF16" s="25">
-        <v>2</v>
-      </c>
-      <c r="AG16" s="25">
-        <v>2</v>
-      </c>
-      <c r="AH16" s="25">
-        <v>2</v>
-      </c>
-      <c r="AI16" s="25">
-        <v>2</v>
-      </c>
-      <c r="AJ16" s="25">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="AB16" s="2">
+        <v>1</v>
+      </c>
+      <c r="AC16" s="2">
+        <v>1</v>
+      </c>
+      <c r="AD16" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE16" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF16" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG16" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH16" s="2">
+        <v>1</v>
+      </c>
+      <c r="AI16" s="2">
+        <v>1</v>
+      </c>
+      <c r="AJ16" s="2">
+        <v>1</v>
       </c>
       <c r="AK16" s="3"/>
       <c r="AL16" s="3"/>
@@ -3742,127 +3745,127 @@
       </c>
       <c r="F23" s="17">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G23" s="17">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H23" s="17">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I23" s="17">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J23" s="17">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K23" s="17">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L23" s="17">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M23" s="17">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N23" s="17">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O23" s="17">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="P23" s="17">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Q23" s="17">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="R23" s="17">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S23" s="17">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="T23" s="17">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="U23" s="17">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="V23" s="17">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="W23" s="17">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="X23" s="17">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Y23" s="17">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Z23" s="17">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AA23" s="17">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AB23" s="17">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AC23" s="17">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AD23" s="17">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AE23" s="17">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AF23" s="17">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AG23" s="17">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AH23" s="17">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AI23" s="17">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AJ23" s="17">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AK23" s="17">
         <f t="shared" si="0"/>
@@ -4380,26 +4383,26 @@
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="F34" s="27"/>
-      <c r="G34" s="37"/>
-      <c r="H34" s="27"/>
-      <c r="I34" s="37"/>
-      <c r="J34" s="27"/>
-      <c r="K34" s="37"/>
-      <c r="L34" s="27"/>
-      <c r="M34" s="37"/>
-      <c r="N34" s="27"/>
-      <c r="O34" s="37"/>
-      <c r="P34" s="27"/>
-      <c r="Q34" s="37"/>
-      <c r="R34" s="27"/>
-      <c r="S34" s="37"/>
-      <c r="T34" s="27"/>
-      <c r="U34" s="37"/>
-      <c r="V34" s="27"/>
-      <c r="W34" s="37"/>
-      <c r="X34" s="27"/>
-      <c r="Y34" s="38"/>
+      <c r="F34" s="52"/>
+      <c r="G34" s="52"/>
+      <c r="H34" s="52"/>
+      <c r="I34" s="52"/>
+      <c r="J34" s="52"/>
+      <c r="K34" s="52"/>
+      <c r="L34" s="52"/>
+      <c r="M34" s="52"/>
+      <c r="N34" s="52"/>
+      <c r="O34" s="52"/>
+      <c r="P34" s="52"/>
+      <c r="Q34" s="52"/>
+      <c r="R34" s="52"/>
+      <c r="S34" s="52"/>
+      <c r="T34" s="52"/>
+      <c r="U34" s="52"/>
+      <c r="V34" s="52"/>
+      <c r="W34" s="52"/>
+      <c r="X34" s="52"/>
+      <c r="Y34" s="52"/>
       <c r="BC34" s="51"/>
       <c r="BD34" s="51"/>
       <c r="BE34" s="51"/>
@@ -4499,16 +4502,16 @@
       <c r="W36" s="31"/>
       <c r="X36" s="28"/>
       <c r="Y36" s="32"/>
-      <c r="AB36" s="30"/>
-      <c r="AC36" s="27"/>
-      <c r="AD36" s="37"/>
-      <c r="AE36" s="27"/>
-      <c r="AF36" s="37"/>
-      <c r="AG36" s="27"/>
-      <c r="AH36" s="37"/>
-      <c r="AI36" s="27"/>
-      <c r="AJ36" s="37"/>
-      <c r="AK36" s="27"/>
+      <c r="AB36" s="52"/>
+      <c r="AC36" s="52"/>
+      <c r="AD36" s="52"/>
+      <c r="AE36" s="52"/>
+      <c r="AF36" s="52"/>
+      <c r="AG36" s="52"/>
+      <c r="AH36" s="52"/>
+      <c r="AI36" s="52"/>
+      <c r="AJ36" s="54"/>
+      <c r="AK36" s="38"/>
       <c r="AL36" s="37"/>
       <c r="AM36" s="27"/>
       <c r="AN36" s="37"/>
@@ -4970,9 +4973,9 @@
       <c r="W40" s="31"/>
       <c r="X40" s="28"/>
       <c r="Y40" s="31"/>
-      <c r="Z40" s="27"/>
-      <c r="AA40" s="30"/>
-      <c r="AB40" s="33"/>
+      <c r="Z40" s="53"/>
+      <c r="AA40" s="54"/>
+      <c r="AB40" s="31"/>
       <c r="AC40" s="28"/>
       <c r="AD40" s="31"/>
       <c r="AE40" s="28"/>
@@ -5346,7 +5349,7 @@
     </row>
     <row r="45" spans="2:130" ht="23.25" x14ac:dyDescent="0.25">
       <c r="T45" s="47" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="48" spans="2:130" x14ac:dyDescent="0.25">
@@ -5726,7 +5729,7 @@
     </row>
     <row r="55" spans="2:130" x14ac:dyDescent="0.25">
       <c r="B55" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="CB55" s="3"/>
       <c r="CC55" s="3"/>
@@ -5808,7 +5811,7 @@
     </row>
     <row r="56" spans="2:130" x14ac:dyDescent="0.25">
       <c r="B56" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="CB56" s="3"/>
       <c r="CC56" s="3"/>
@@ -5986,43 +5989,43 @@
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
       <c r="F59" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G59" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H59" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I59" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J59" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K59" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L59" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M59" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N59" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O59" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P59" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q59" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R59" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S59" s="3"/>
       <c r="T59" s="3"/>
@@ -6233,58 +6236,58 @@
       <c r="Q61" s="3"/>
       <c r="R61" s="3"/>
       <c r="Z61" s="24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AA61" s="24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB61" s="24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AC61" s="24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AD61" s="24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE61" s="24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AF61" s="24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AG61" s="24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AH61" s="24">
-        <v>2</v>
-      </c>
-      <c r="AI61" s="53">
-        <v>2</v>
-      </c>
-      <c r="AJ61" s="53">
-        <v>2</v>
-      </c>
-      <c r="AK61" s="53">
-        <v>2</v>
-      </c>
-      <c r="AL61" s="53">
-        <v>2</v>
-      </c>
-      <c r="AM61" s="53">
-        <v>2</v>
-      </c>
-      <c r="AN61" s="53">
-        <v>2</v>
-      </c>
-      <c r="AO61" s="53">
-        <v>2</v>
-      </c>
-      <c r="AP61" s="53">
-        <v>2</v>
-      </c>
-      <c r="AQ61" s="53">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="AI61" s="24">
+        <v>1</v>
+      </c>
+      <c r="AJ61" s="24">
+        <v>1</v>
+      </c>
+      <c r="AK61" s="24">
+        <v>1</v>
+      </c>
+      <c r="AL61" s="24">
+        <v>1</v>
+      </c>
+      <c r="AM61" s="24">
+        <v>1</v>
+      </c>
+      <c r="AN61" s="24">
+        <v>1</v>
+      </c>
+      <c r="AO61" s="24">
+        <v>1</v>
+      </c>
+      <c r="AP61" s="24">
+        <v>1</v>
+      </c>
+      <c r="AQ61" s="24">
+        <v>1</v>
       </c>
       <c r="AR61" s="3"/>
       <c r="AS61" s="3"/>
@@ -6859,55 +6862,55 @@
       </c>
       <c r="F68" s="17">
         <f t="shared" ref="F68" si="6">SUM(F48:F67)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G68" s="17">
         <f t="shared" ref="G68" si="7">SUM(G48:G67)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H68" s="17">
         <f t="shared" ref="H68" si="8">SUM(H48:H67)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I68" s="17">
         <f t="shared" ref="I68" si="9">SUM(I48:I67)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J68" s="17">
         <f t="shared" ref="J68" si="10">SUM(J48:J67)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K68" s="17">
         <f t="shared" ref="K68" si="11">SUM(K48:K67)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L68" s="17">
         <f t="shared" ref="L68" si="12">SUM(L48:L67)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M68" s="17">
         <f t="shared" ref="M68" si="13">SUM(M48:M67)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N68" s="17">
         <f t="shared" ref="N68" si="14">SUM(N48:N67)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O68" s="17">
         <f t="shared" ref="O68" si="15">SUM(O48:O67)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="P68" s="17">
         <f t="shared" ref="P68" si="16">SUM(P48:P67)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Q68" s="17">
         <f t="shared" ref="Q68" si="17">SUM(Q48:Q67)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="R68" s="17">
         <f t="shared" ref="R68" si="18">SUM(R48:R67)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S68" s="17">
         <f t="shared" ref="S68" si="19">SUM(S48:S67)</f>
@@ -6939,75 +6942,75 @@
       </c>
       <c r="Z68" s="17">
         <f t="shared" ref="Z68" si="26">SUM(Z48:Z67)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AA68" s="17">
         <f t="shared" ref="AA68" si="27">SUM(AA48:AA67)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AB68" s="17">
         <f t="shared" ref="AB68" si="28">SUM(AB48:AB67)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AC68" s="17">
         <f t="shared" ref="AC68" si="29">SUM(AC48:AC67)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AD68" s="17">
         <f t="shared" ref="AD68" si="30">SUM(AD48:AD67)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AE68" s="17">
         <f t="shared" ref="AE68" si="31">SUM(AE48:AE67)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AF68" s="17">
         <f t="shared" ref="AF68" si="32">SUM(AF48:AF67)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AG68" s="17">
         <f t="shared" ref="AG68" si="33">SUM(AG48:AG67)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AH68" s="17">
         <f t="shared" ref="AH68" si="34">SUM(AH48:AH67)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AI68" s="17">
         <f t="shared" ref="AI68" si="35">SUM(AI48:AI67)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AJ68" s="17">
         <f t="shared" ref="AJ68" si="36">SUM(AJ48:AJ67)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AK68" s="17">
         <f t="shared" ref="AK68" si="37">SUM(AK48:AK67)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AL68" s="17">
         <f t="shared" ref="AL68" si="38">SUM(AL48:AL67)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AM68" s="17">
         <f t="shared" ref="AM68" si="39">SUM(AM48:AM67)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AN68" s="17">
         <f t="shared" ref="AN68" si="40">SUM(AN48:AN67)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AO68" s="17">
         <f t="shared" ref="AO68" si="41">SUM(AO48:AO67)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AP68" s="17">
         <f t="shared" ref="AP68" si="42">SUM(AP48:AP67)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AQ68" s="17">
         <f t="shared" ref="AQ68" si="43">SUM(AQ48:AQ67)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AR68" s="17">
         <f t="shared" ref="AR68" si="44">SUM(AR48:AR67)</f>
@@ -7736,19 +7739,19 @@
         <f t="shared" si="132"/>
         <v>9</v>
       </c>
-      <c r="F80" s="27"/>
-      <c r="G80" s="37"/>
-      <c r="H80" s="27"/>
-      <c r="I80" s="37"/>
-      <c r="J80" s="27"/>
-      <c r="K80" s="37"/>
-      <c r="L80" s="27"/>
-      <c r="M80" s="37"/>
-      <c r="N80" s="27"/>
-      <c r="O80" s="37"/>
-      <c r="P80" s="27"/>
-      <c r="Q80" s="37"/>
-      <c r="R80" s="27"/>
+      <c r="F80" s="52"/>
+      <c r="G80" s="52"/>
+      <c r="H80" s="52"/>
+      <c r="I80" s="52"/>
+      <c r="J80" s="52"/>
+      <c r="K80" s="52"/>
+      <c r="L80" s="52"/>
+      <c r="M80" s="52"/>
+      <c r="N80" s="52"/>
+      <c r="O80" s="52"/>
+      <c r="P80" s="52"/>
+      <c r="Q80" s="52"/>
+      <c r="R80" s="52"/>
       <c r="S80" s="51"/>
       <c r="T80" s="51"/>
       <c r="U80" s="51"/>
@@ -7857,22 +7860,22 @@
       <c r="W82" s="37"/>
       <c r="X82" s="27"/>
       <c r="Y82" s="38"/>
-      <c r="AB82" s="30"/>
-      <c r="AC82" s="27"/>
-      <c r="AD82" s="37"/>
-      <c r="AE82" s="27"/>
-      <c r="AF82" s="37"/>
-      <c r="AG82" s="27"/>
-      <c r="AH82" s="37"/>
-      <c r="AI82" s="27"/>
-      <c r="AJ82" s="37"/>
-      <c r="AK82" s="27"/>
-      <c r="AL82" s="37"/>
-      <c r="AM82" s="27"/>
-      <c r="AN82" s="37"/>
-      <c r="AO82" s="27"/>
-      <c r="AP82" s="37"/>
-      <c r="AQ82" s="27"/>
+      <c r="AB82" s="52"/>
+      <c r="AC82" s="52"/>
+      <c r="AD82" s="52"/>
+      <c r="AE82" s="52"/>
+      <c r="AF82" s="52"/>
+      <c r="AG82" s="52"/>
+      <c r="AH82" s="52"/>
+      <c r="AI82" s="52"/>
+      <c r="AJ82" s="52"/>
+      <c r="AK82" s="52"/>
+      <c r="AL82" s="52"/>
+      <c r="AM82" s="52"/>
+      <c r="AN82" s="52"/>
+      <c r="AO82" s="52"/>
+      <c r="AP82" s="52"/>
+      <c r="AQ82" s="52"/>
       <c r="AR82" s="51"/>
       <c r="AS82" s="51"/>
       <c r="AT82" s="51"/>
@@ -8329,9 +8332,9 @@
       <c r="W86" s="31"/>
       <c r="X86" s="28"/>
       <c r="Y86" s="31"/>
-      <c r="Z86" s="27"/>
-      <c r="AA86" s="30"/>
-      <c r="AB86" s="33"/>
+      <c r="Z86" s="53"/>
+      <c r="AA86" s="54"/>
+      <c r="AB86" s="31"/>
       <c r="AC86" s="28"/>
       <c r="AD86" s="31"/>
       <c r="AE86" s="28"/>

</xml_diff>